<commit_message>
Add records to db
</commit_message>
<xml_diff>
--- a/static/db/narratives_db.xlsx
+++ b/static/db/narratives_db.xlsx
@@ -10,6 +10,10 @@
     <sheet name="wild" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Test Sheet" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Integration Test" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Test Topic Add Narrative" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Duplicate Test Topic" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Test Topic" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="ssss" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -644,7 +648,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -694,7 +698,7 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://example.com/test-video-1749316131</t>
+          <t>https://example.com/test-video-1749324268</t>
         </is>
       </c>
     </row>
@@ -732,7 +736,7 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://example.com/test-video-1749316205</t>
+          <t>https://example.com/test-video-1749324338</t>
         </is>
       </c>
     </row>
@@ -751,7 +755,216 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://example.com/test-video-1749316276</t>
+          <t>https://example.com/test-video-1749324427</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Test narrative for comprehensive testing</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Test story content</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://example.com/test-video-1749324483</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Test narrative for comprehensive testing</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Test story content</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://example.com/test-video-1749324740</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Test narrative for comprehensive testing</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Test story content</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://example.com/test-video-1749324853</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Test narrative for comprehensive testing</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Test story content</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://example.com/test-video-1749324872</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Test narrative for comprehensive testing</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Test story content</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://example.com/test-video-1749325030</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Test narrative for comprehensive testing</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Test story content</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://example.com/test-video-1749325581</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Test narrative for comprehensive testing</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Test story content</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>https://example.com/test-video-1749325633</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Test narrative for comprehensive testing</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Test story content</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://example.com/test-video-1749326680</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Test narrative for comprehensive testing</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Test story content</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>https://example.com/test-video-1749326742</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Test narrative for comprehensive testing</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Test story content</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://example.com/test-video-1749326937</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Test narrative for comprehensive testing</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Test story content</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>https://example.com/test-video-1749326999</t>
         </is>
       </c>
     </row>
@@ -766,7 +979,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -816,7 +1029,7 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://example.com/integration-test-1749316131</t>
+          <t>https://example.com/integration-test-1749324268</t>
         </is>
       </c>
     </row>
@@ -835,7 +1048,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://example.com/integration-test-1749316205</t>
+          <t>https://example.com/integration-test-1749324338</t>
         </is>
       </c>
     </row>
@@ -854,7 +1067,848 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://example.com/integration-test-1749316276</t>
+          <t>https://example.com/integration-test-1749324427</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Integration test narrative</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Integration test story</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://example.com/integration-test-1749324483</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Integration test narrative</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Integration test story</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Nir Kon</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://example.com/integration-test-1749324741</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Integration test narrative</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Integration test story</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://example.com/integration-test-1749324853</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Integration test narrative</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Integration test story</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://example.com/integration-test-1749324872</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Integration test narrative</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Integration test story</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://example.com/integration-test-1749325031</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Integration test narrative</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Integration test story</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://example.com/integration-test-1749325581</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Integration test narrative</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Integration test story</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://example.com/integration-test-1749325633</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Integration test narrative</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Integration test story</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>https://example.com/integration-test-1749326680</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Integration test narrative</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Integration test story</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://example.com/integration-test-1749326742</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Integration test narrative</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Integration test story</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>https://example.com/integration-test-1749326937</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Integration test narrative</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Integration test story</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://example.com/integration-test-1749326999</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Narrative</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Story</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Tagger_1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tagger_1_Result</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Test narrative for add endpoint</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>This is a test story for the add narrative endpoint functionality</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://example.com/test-add-narrative-9109683475687634795</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Test narrative for add endpoint</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>This is a test story for the add narrative endpoint functionality</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://example.com/test-add-narrative-8875983319858039013</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Test narrative for add endpoint</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>This is a test story for the add narrative endpoint functionality</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://example.com/test-add-narrative--4022726412704695955</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Test narrative for add endpoint</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>This is a test story for the add narrative endpoint functionality</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://example.com/test-add-narrative-2693365805858967044</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Test narrative for add endpoint</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>This is a test story for the add narrative endpoint functionality</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://example.com/test-add-narrative--4196134297481682363</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Test narrative for add endpoint</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>This is a test story for the add narrative endpoint functionality</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://example.com/test-add-narrative-1222646142236062237</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Test narrative for add endpoint</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>This is a test story for the add narrative endpoint functionality</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://example.com/test-add-narrative-7843454298559033762</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Test narrative for add endpoint</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>This is a test story for the add narrative endpoint functionality</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://example.com/test-add-narrative-3999583981817640447</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Test narrative for add endpoint</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>This is a test story for the add narrative endpoint functionality</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://example.com/test-add-narrative--1694519282609914268</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Test narrative for add endpoint</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>This is a test story for the add narrative endpoint functionality</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://example.com/test-add-narrative--2610078888296625328</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Narrative</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Story</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Tagger_1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tagger_1_Result</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Duplicate test narrative</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Test story for duplicate link test</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://example.com/duplicate-test-link</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Narrative</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Story</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Tagger_1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tagger_1_Result</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Test narrative</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Test story</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>not-a-url</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Test narrative</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Test story</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ftp://example.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Test narrative</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Test story</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>http://</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Test narrative</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Test story</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Test narrative</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Test story</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Test narrative</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Test story</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Test narrative</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Test story</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Test add narrative functionality</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>This is a comprehensive test of the add narrative endpoint</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://example.com/test-add-narrative-endpoint</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Test narrative</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Test story</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Narrative</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Story</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Tagger_1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tagger_1_Result</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>sadasda</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>fdgdfvvsseee</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>http://localhost:8000/tagging-management544354353</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sadasda</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>dsfadsfsadfa</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>http://localhost:8000/tagging-managementdfsdfsd</t>
         </is>
       </c>
     </row>

</xml_diff>